<commit_message>
Made calc adjacency and calc target functions work. One small bug left to fix with doorways.
</commit_message>
<xml_diff>
--- a/ClueBoardLayout.xlsx
+++ b/ClueBoardLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\Desktop\Software Engineering\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\EclipseProjects\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="64" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
started on JFrame to display everything
</commit_message>
<xml_diff>
--- a/ClueBoardLayout.xlsx
+++ b/ClueBoardLayout.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\Desktop\Software Engineering\ClueGame\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13425" windowHeight="7425"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18570" windowHeight="5790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="31">
   <si>
     <t>W</t>
   </si>
@@ -114,6 +110,9 @@
   </si>
   <si>
     <t>Dark Blue: Test Targets</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -231,259 +230,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -830,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
-      <selection activeCell="AB22" sqref="AB22"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="64" workbookViewId="0">
+      <selection activeCell="AC23" sqref="AC23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="W11" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X11" t="s">
         <v>0</v>
@@ -3821,20 +3568,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AD1 AD32:AD51 A10:AD11 B8:W8 Y8:AD8 A29:E29 A28:D28 AB28:AD28 B24:N24 A23:AB23 AD23 A15:W15 A13:X13 AA13:AD13 A20:J20 A19:U19 W19:AD19 A26:B26 A25 U25:AD25 A14:J14 M14 P14:AD14 A22:AD22 A21:L21 O21:AD21 A30:F30 H30:AC30 G29:AD29 F28:T28 A27:C27 E27:AD27 D26:AD26 D25 A18:AD18 A17:B17 D16:W16 A7:F7 D5:L5 A4:AD4 A2:B2 D2:AD2 B16 A9:AB9 AD9 N5:AD5 E17:N17 A5:B6 D6:AD6 Y15:AD16 P24:Z24 F25:S25 H7:AD7 V28:Z28 A12:AC12 A3:E3 U3:AD3 G3:S3 L20:AD20 P17:AD17 AB24:AD24">
-    <cfRule type="containsText" dxfId="39" priority="2" stopIfTrue="1" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="3" priority="2" stopIfTrue="1" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="1" stopIfTrue="1" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="2" priority="1" stopIfTrue="1" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:AD2 AD32:AD51 H10:AD11 H8:W8 Y8:AD8 H29:AD29 H28:T28 AB28:AD28 H24:N24 H23:AB23 AD23 H13:X13 AA13:AD13 H20:J20 H19:U19 W19:AD19 H26:AD27 H25:S25 U25:AD25 H14:J14 M14 P14:AD14 H22:AD22 H21:L21 O21:AD21 H9:AB9 AD9 H6:AD7 H5:L5 N5:AD5 H18:AD18 H15:W16 Y15:AD16 P24:Z24 V28:Z28 H12:AC12 H4:AD4 H3:S3 U3:AD3 L20:AD20 H30:AC30 H17:N17 P17:AD17 AB24:AD24">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="4">
       <formula>LEN(TRIM(H1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1 A30:F30 A29:E29 G29 A28:D28 F28:G28 A27:C27 E27:G27 A26:B26 A25 D26:G26 B24:G24 A18:G23 A17:B17 D16:G16 A9:G15 A4:G4 A2:B2 D2:G2 B16 E17:G17 A5:B6 D5:G6 D25 F25:G25 A7:F7 B8:G8 A3:E3 G3">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Created board panel so the game board shows up on the GUI
</commit_message>
<xml_diff>
--- a/ClueBoardLayout.xlsx
+++ b/ClueBoardLayout.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\EclipseProjects\ClueGame\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18570" windowHeight="5790"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="40">
   <si>
     <t>W</t>
   </si>
@@ -113,6 +117,33 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>DN</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>LN</t>
+  </si>
+  <si>
+    <t>QN</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>ON</t>
   </si>
 </sst>
 </file>
@@ -577,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="64" workbookViewId="0">
-      <selection activeCell="AC23" sqref="AC23"/>
+    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
+      <selection activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +809,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -948,7 +979,7 @@
         <v>8</v>
       </c>
       <c r="AA4" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="AB4" t="s">
         <v>8</v>
@@ -998,7 +1029,7 @@
         <v>5</v>
       </c>
       <c r="L5" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>5</v>
@@ -1972,7 +2003,7 @@
         <v>0</v>
       </c>
       <c r="T15" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="U15" t="s">
         <v>19</v>
@@ -1990,7 +2021,7 @@
         <v>22</v>
       </c>
       <c r="Z15" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="AA15" t="s">
         <v>22</v>
@@ -2105,7 +2136,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3150,7 +3181,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
@@ -3278,7 +3309,7 @@
         <v>15</v>
       </c>
       <c r="L29" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="M29" t="s">
         <v>15</v>
@@ -3320,7 +3351,7 @@
         <v>17</v>
       </c>
       <c r="Z29" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="AA29" t="s">
         <v>17</v>

</xml_diff>